<commit_message>
working on model training
</commit_message>
<xml_diff>
--- a/6_CYBERSECURITY_CHATBOT/data/security_faq.xlsx
+++ b/6_CYBERSECURITY_CHATBOT/data/security_faq.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
-    <t xml:space="preserve">QUESTION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANSWER</t>
+    <t xml:space="preserve">Question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer</t>
   </si>
   <si>
     <t xml:space="preserve">Why do I need to worry about Cyber Security?</t>
@@ -481,7 +481,7 @@
   <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>